<commit_message>
done with figure legends
</commit_message>
<xml_diff>
--- a/Tables/Table 4 - ZmIonome HPO Genes.xlsx
+++ b/Tables/Table 4 - ZmIonome HPO Genes.xlsx
@@ -398,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,6 +466,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,7 +770,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,43 +782,43 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="L2" s="25"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
@@ -825,72 +828,72 @@
         <v>5</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="J3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="D4" s="9">
         <v>13</v>
       </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
       <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
         <v>13</v>
       </c>
+      <c r="G4" s="9">
+        <v>56</v>
+      </c>
       <c r="H4" s="9">
-        <v>56</v>
-      </c>
-      <c r="I4" s="9">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="15">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15">
         <v>57</v>
       </c>
-      <c r="L4" s="3">
-        <v>69</v>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -898,37 +901,37 @@
         <v>11</v>
       </c>
       <c r="B5" s="4">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
         <v>27</v>
       </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
       <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
         <v>27</v>
       </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
       <c r="H5" s="10">
         <v>1</v>
       </c>
-      <c r="I5" s="10">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="15">
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
         <v>2</v>
       </c>
-      <c r="L5" s="4">
-        <v>28</v>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -936,37 +939,37 @@
         <v>12</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
         <v>0</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="10">
         <v>0</v>
       </c>
       <c r="H6" s="10">
-        <v>0</v>
-      </c>
-      <c r="I6" s="10">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="15">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="15">
         <v>2</v>
       </c>
-      <c r="L6" s="4">
-        <v>2</v>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -974,37 +977,37 @@
         <v>13</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
       </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
         <v>0</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="10">
         <v>0</v>
       </c>
       <c r="H7" s="10">
-        <v>0</v>
-      </c>
-      <c r="I7" s="10">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
         <v>2</v>
       </c>
-      <c r="K7" s="15">
+      <c r="J7" s="15">
         <v>3</v>
       </c>
-      <c r="L7" s="4">
-        <v>3</v>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1012,37 +1015,37 @@
         <v>14</v>
       </c>
       <c r="B8" s="4">
+        <v>209</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>126</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>126</v>
+      </c>
+      <c r="G8" s="10">
+        <v>97</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <v>98</v>
+      </c>
+      <c r="K8" s="4">
         <v>15</v>
       </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
-        <v>126</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>126</v>
-      </c>
-      <c r="H8" s="10">
-        <v>97</v>
-      </c>
-      <c r="I8" s="10">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="15">
-        <v>98</v>
-      </c>
-      <c r="L8" s="4">
-        <v>209</v>
+      <c r="L8" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1050,37 +1053,37 @@
         <v>15</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
       </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10">
+      <c r="D9" s="10">
         <v>26</v>
       </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
       <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
         <v>26</v>
       </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
       <c r="H9" s="10">
         <v>0</v>
       </c>
-      <c r="I9" s="10">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="15">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>26</v>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1088,37 +1091,37 @@
         <v>16</v>
       </c>
       <c r="B10" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
       </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10">
+      <c r="D10" s="10">
         <v>11</v>
       </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
       <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="7">
         <v>11</v>
       </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
       <c r="H10" s="10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="15">
-        <v>1</v>
-      </c>
-      <c r="L10" s="4">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1126,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="B11" s="4">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
       </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="10">
         <v>15</v>
       </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
       <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7">
         <v>15</v>
       </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
       <c r="H11" s="10">
         <v>0</v>
       </c>
-      <c r="I11" s="10">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="I11" s="1">
         <v>2</v>
       </c>
-      <c r="K11" s="15">
+      <c r="J11" s="15">
         <v>2</v>
       </c>
-      <c r="L11" s="4">
-        <v>17</v>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1164,37 +1167,37 @@
         <v>18</v>
       </c>
       <c r="B12" s="4">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
       </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10">
-        <v>1</v>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
       </c>
       <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>24</v>
       </c>
       <c r="H12" s="10">
-        <v>24</v>
-      </c>
-      <c r="I12" s="10">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>1</v>
-      </c>
-      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="15">
         <v>25</v>
       </c>
-      <c r="L12" s="4">
-        <v>26</v>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1202,37 +1205,37 @@
         <v>19</v>
       </c>
       <c r="B13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
       </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
         <v>0</v>
       </c>
       <c r="F13" s="7">
         <v>0</v>
       </c>
-      <c r="G13" s="7">
-        <v>0</v>
+      <c r="G13" s="10">
+        <v>1</v>
       </c>
       <c r="H13" s="10">
         <v>1</v>
       </c>
-      <c r="I13" s="10">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="15">
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
         <v>2</v>
       </c>
-      <c r="L13" s="4">
-        <v>2</v>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1240,37 +1243,37 @@
         <v>20</v>
       </c>
       <c r="B14" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
       </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10">
-        <v>1</v>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
       </c>
       <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="G14" s="10">
+        <v>6</v>
       </c>
       <c r="H14" s="10">
-        <v>6</v>
-      </c>
-      <c r="I14" s="10">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="15">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15">
         <v>7</v>
       </c>
-      <c r="L14" s="4">
-        <v>8</v>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1278,37 +1281,37 @@
         <v>21</v>
       </c>
       <c r="B15" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15" s="7">
         <v>0</v>
       </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
         <v>0</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
       </c>
-      <c r="G15" s="7">
-        <v>0</v>
+      <c r="G15" s="10">
+        <v>1</v>
       </c>
       <c r="H15" s="10">
-        <v>1</v>
-      </c>
-      <c r="I15" s="10">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-      <c r="K15" s="15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="15">
         <v>2</v>
       </c>
-      <c r="L15" s="4">
-        <v>2</v>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1316,37 +1319,37 @@
         <v>22</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
       </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="10">
-        <v>0</v>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>16</v>
       </c>
       <c r="F16" s="7">
         <v>16</v>
       </c>
-      <c r="G16" s="7">
-        <v>16</v>
+      <c r="G16" s="10">
+        <v>0</v>
       </c>
       <c r="H16" s="10">
-        <v>0</v>
-      </c>
-      <c r="I16" s="10">
         <v>3</v>
       </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="15">
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
         <v>3</v>
       </c>
-      <c r="L16" s="4">
-        <v>18</v>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1354,37 +1357,37 @@
         <v>23</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
       </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="10">
-        <v>0</v>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>52</v>
       </c>
       <c r="F17" s="7">
         <v>52</v>
       </c>
-      <c r="G17" s="7">
-        <v>52</v>
+      <c r="G17" s="10">
+        <v>0</v>
       </c>
       <c r="H17" s="10">
         <v>0</v>
       </c>
-      <c r="I17" s="10">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="15">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
-        <v>52</v>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1392,37 +1395,37 @@
         <v>24</v>
       </c>
       <c r="B18" s="4">
+        <v>105</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10">
+        <v>76</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>76</v>
+      </c>
+      <c r="G18" s="10">
+        <v>34</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="15">
+        <v>35</v>
+      </c>
+      <c r="K18" s="4">
         <v>6</v>
       </c>
-      <c r="C18" s="7">
-        <v>0</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="10">
-        <v>76</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="7">
-        <v>76</v>
-      </c>
-      <c r="H18" s="10">
-        <v>34</v>
-      </c>
-      <c r="I18" s="10">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="15">
-        <v>35</v>
-      </c>
-      <c r="L18" s="4">
-        <v>105</v>
+      <c r="L18" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1430,37 +1433,37 @@
         <v>25</v>
       </c>
       <c r="B19" s="4">
+        <v>60</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>58</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
+        <v>58</v>
+      </c>
+      <c r="G19" s="10">
+        <v>4</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15">
+        <v>4</v>
+      </c>
+      <c r="K19" s="4">
         <v>2</v>
       </c>
-      <c r="C19" s="7">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10">
-        <v>58</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="7">
-        <v>58</v>
-      </c>
-      <c r="H19" s="10">
-        <v>4</v>
-      </c>
-      <c r="I19" s="10">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
-      <c r="K19" s="15">
-        <v>4</v>
-      </c>
-      <c r="L19" s="4">
-        <v>60</v>
+      <c r="L19" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1468,82 +1471,82 @@
         <v>26</v>
       </c>
       <c r="B20" s="5">
+        <v>49</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>8</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>8</v>
+      </c>
+      <c r="G20" s="11">
+        <v>43</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="16">
+        <v>4</v>
+      </c>
+      <c r="K20" s="5">
         <v>2</v>
       </c>
-      <c r="C20" s="8">
-        <v>0</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="11">
+      <c r="L20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="22">
+        <v>610</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0</v>
+      </c>
+      <c r="D21" s="19">
+        <v>326</v>
+      </c>
+      <c r="E21" s="18">
+        <v>66</v>
+      </c>
+      <c r="F21" s="18">
+        <v>391</v>
+      </c>
+      <c r="G21" s="19">
+        <v>228</v>
+      </c>
+      <c r="H21" s="19">
+        <v>11</v>
+      </c>
+      <c r="I21" s="20">
         <v>8</v>
       </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <v>8</v>
-      </c>
-      <c r="H20" s="11">
-        <v>43</v>
-      </c>
-      <c r="I20" s="11">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="16">
-        <v>4</v>
-      </c>
-      <c r="L20" s="5">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="17">
+      <c r="J21" s="21">
+        <v>247</v>
+      </c>
+      <c r="K21" s="17">
         <v>26</v>
       </c>
-      <c r="C21" s="18">
+      <c r="L21" s="18">
         <v>2</v>
-      </c>
-      <c r="D21" s="18">
-        <v>0</v>
-      </c>
-      <c r="E21" s="19">
-        <v>326</v>
-      </c>
-      <c r="F21" s="18">
-        <v>66</v>
-      </c>
-      <c r="G21" s="18">
-        <v>391</v>
-      </c>
-      <c r="H21" s="19">
-        <v>228</v>
-      </c>
-      <c r="I21" s="19">
-        <v>11</v>
-      </c>
-      <c r="J21" s="20">
-        <v>8</v>
-      </c>
-      <c r="K21" s="21">
-        <v>247</v>
-      </c>
-      <c r="L21" s="22">
-        <v>610</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C2:F2"/>
     <mergeCell ref="B1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:L21">

</xml_diff>